<commit_message>
Adding of files for Waste management and Energy efficiencies and creation of separate Graph-scripts
</commit_message>
<xml_diff>
--- a/Data/4_PY_EoL_RecoveryRate_V2.0.xlsx
+++ b/Data/4_PY_EoL_RecoveryRate_V2.0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="141">
   <si>
     <t>Date created</t>
   </si>
@@ -96,12 +96,6 @@
     <t># Two types are supported: list and table</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>SSP_Regions_32</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -346,6 +340,105 @@
   </si>
   <si>
     <t>4_PY_EoL_RecoveryRate</t>
+  </si>
+  <si>
+    <t>solar photovoltaic power plant</t>
+  </si>
+  <si>
+    <t>concentrating solar power plant (CSP)</t>
+  </si>
+  <si>
+    <t>wind power plant onshore</t>
+  </si>
+  <si>
+    <t>wind power plant offshore</t>
+  </si>
+  <si>
+    <t>hydro power plant</t>
+  </si>
+  <si>
+    <t>nuclear power plant</t>
+  </si>
+  <si>
+    <t>coal power plant</t>
+  </si>
+  <si>
+    <t>coal power plant without abatement measures</t>
+  </si>
+  <si>
+    <t>bio powerplant</t>
+  </si>
+  <si>
+    <t>oil power plant</t>
+  </si>
+  <si>
+    <t>geothermal power plant</t>
+  </si>
+  <si>
+    <t>IGCC power plant</t>
+  </si>
+  <si>
+    <t>light oil combined cycle</t>
+  </si>
+  <si>
+    <t>gas combined cycle power plant</t>
+  </si>
+  <si>
+    <t>advanced coal power plant with CCS</t>
+  </si>
+  <si>
+    <t>coal power plant with CCS</t>
+  </si>
+  <si>
+    <t>biomass power plant with CCS</t>
+  </si>
+  <si>
+    <t>gas combined cycle power plant with CCS</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Air-cooler</t>
+  </si>
+  <si>
+    <t>Air-conditioning</t>
+  </si>
+  <si>
+    <t>Refridgerator</t>
+  </si>
+  <si>
+    <t>Microwave</t>
+  </si>
+  <si>
+    <t>Washing Machine</t>
+  </si>
+  <si>
+    <t>Tumble dryer</t>
+  </si>
+  <si>
+    <t>Dish washer</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>VCR/DVD player</t>
+  </si>
+  <si>
+    <t>PC &amp; Laptop computers</t>
+  </si>
+  <si>
+    <t>Other small appliances</t>
+  </si>
+  <si>
+    <t>#1 Copper scrap</t>
+  </si>
+  <si>
+    <t>SSP_Regions_1</t>
+  </si>
+  <si>
+    <t>Region world</t>
   </si>
 </sst>
 </file>
@@ -538,8 +631,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -843,11 +936,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.109375" customWidth="1"/>
@@ -862,13 +955,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -876,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -891,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
@@ -906,7 +999,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
@@ -921,43 +1014,43 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L7" s="1"/>
     </row>
@@ -966,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
@@ -981,13 +1074,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L9" s="1"/>
     </row>
@@ -996,7 +1089,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
@@ -1056,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
@@ -1071,7 +1164,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
@@ -1083,7 +1176,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
@@ -1092,7 +1185,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1101,7 +1194,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -1110,7 +1203,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1119,7 +1212,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -1131,13 +1224,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="20">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>24</v>
@@ -1149,16 +1242,16 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>24</v>
@@ -1170,16 +1263,16 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>24</v>
@@ -1187,22 +1280,22 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>24</v>
@@ -1210,22 +1303,22 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>24</v>
@@ -1233,22 +1326,22 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>24</v>
@@ -1256,16 +1349,16 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>24</v>
@@ -1383,10 +1476,10 @@
   <dimension ref="A1:L481"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E6:E7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
@@ -1401,1181 +1494,1181 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F2">
         <v>69</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F3">
         <v>69</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4">
         <v>69</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5">
         <v>69</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6">
         <v>69</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7">
         <v>69</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8">
         <v>93</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9">
         <v>93</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10">
         <v>93</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11">
         <v>93</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12">
         <v>93</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F13">
         <v>93</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F14">
         <v>93</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F15">
         <v>93</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F16">
         <v>93</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17">
         <v>93</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F18">
         <v>93</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F19">
         <v>93</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F20">
         <v>93</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F21">
         <v>93</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F22">
         <v>93</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F23">
         <v>100</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F24">
         <v>100</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F25">
         <v>100</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F26">
         <v>100</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F27">
         <v>100</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F28">
         <v>100</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F29">
         <v>100</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F30">
         <v>100</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F31">
         <v>100</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F32">
         <v>87</v>
       </c>
       <c r="G32" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" t="s">
         <v>70</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F33">
         <v>87</v>
       </c>
       <c r="G33" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" t="s">
         <v>70</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" t="s">
-        <v>72</v>
       </c>
       <c r="K33" s="9"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F34">
         <v>87</v>
       </c>
       <c r="G34" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" t="s">
         <v>70</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" t="s">
-        <v>72</v>
       </c>
       <c r="K34" s="9"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F35">
         <v>87</v>
       </c>
       <c r="G35" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" t="s">
         <v>70</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" t="s">
-        <v>72</v>
       </c>
       <c r="K35" s="9"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F36">
         <v>87</v>
       </c>
       <c r="G36" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" t="s">
         <v>70</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" t="s">
-        <v>72</v>
       </c>
       <c r="K36" s="9"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F37">
         <v>87</v>
       </c>
       <c r="G37" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" t="s">
         <v>70</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" t="s">
-        <v>72</v>
       </c>
       <c r="K37" s="9"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F38">
         <v>87</v>
       </c>
       <c r="G38" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" t="s">
         <v>70</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" t="s">
-        <v>72</v>
       </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F39">
         <v>87</v>
       </c>
       <c r="G39" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
         <v>70</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" t="s">
-        <v>72</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F40">
         <v>87</v>
       </c>
       <c r="G40" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I40" t="s">
         <v>70</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" t="s">
-        <v>72</v>
       </c>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -2583,31 +2676,31 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F41">
         <v>78</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -2615,31 +2708,31 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F42">
         <v>78</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
@@ -2647,31 +2740,31 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F43">
         <v>78</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
@@ -2679,31 +2772,31 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F44">
         <v>78</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -2711,31 +2804,31 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F45">
         <v>78</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
@@ -2743,31 +2836,31 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F46">
         <v>78</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -2775,31 +2868,31 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F47">
         <v>78</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -2807,31 +2900,31 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D48" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F48">
         <v>78</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2839,31 +2932,31 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F49">
         <v>78</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I49" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -2871,31 +2964,31 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F50">
         <v>87.5</v>
       </c>
       <c r="G50" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" t="s">
         <v>70</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I50" t="s">
-        <v>72</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
@@ -2903,31 +2996,31 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F51">
         <v>87.5</v>
       </c>
       <c r="G51" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I51" t="s">
         <v>70</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I51" t="s">
-        <v>72</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -2935,31 +3028,31 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F52">
         <v>87.5</v>
       </c>
       <c r="G52" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I52" t="s">
         <v>70</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" t="s">
-        <v>72</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -2967,31 +3060,31 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F53">
         <v>87.5</v>
       </c>
       <c r="G53" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I53" t="s">
         <v>70</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I53" t="s">
-        <v>72</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -2999,31 +3092,31 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F54">
         <v>87.5</v>
       </c>
       <c r="G54" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I54" t="s">
         <v>70</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I54" t="s">
-        <v>72</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -3031,31 +3124,31 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F55">
         <v>87.5</v>
       </c>
       <c r="G55" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I55" t="s">
         <v>70</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" t="s">
-        <v>72</v>
       </c>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -3063,31 +3156,31 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F56">
         <v>87.5</v>
       </c>
       <c r="G56" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I56" t="s">
         <v>70</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I56" t="s">
-        <v>72</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -3095,31 +3188,31 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E57" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F57">
         <v>87.5</v>
       </c>
       <c r="G57" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I57" t="s">
         <v>70</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I57" t="s">
-        <v>72</v>
       </c>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -3127,31 +3220,31 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F58">
         <v>87.5</v>
       </c>
       <c r="G58" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I58" t="s">
         <v>70</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I58" t="s">
-        <v>72</v>
       </c>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
@@ -3159,31 +3252,31 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E59" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F59">
         <v>87.5</v>
       </c>
       <c r="G59" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I59" t="s">
         <v>70</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I59" t="s">
-        <v>72</v>
       </c>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -3191,31 +3284,31 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F60">
         <v>87.5</v>
       </c>
       <c r="G60" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I60" t="s">
         <v>70</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I60" t="s">
-        <v>72</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
@@ -3223,31 +3316,31 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F61">
         <v>87.5</v>
       </c>
       <c r="G61" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I61" t="s">
         <v>70</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I61" t="s">
-        <v>72</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
@@ -3255,31 +3348,31 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F62">
         <v>67</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I62" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
@@ -3287,31 +3380,31 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E63" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F63">
         <v>67</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H63" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
@@ -3319,31 +3412,31 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F64">
         <v>67</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I64" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
@@ -3351,31 +3444,31 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F65">
         <v>67</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I65" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
@@ -3383,100 +3476,931 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E66" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F66">
         <v>67</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D67" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F67">
         <v>67</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H67" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I67" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B68" s="9"/>
-      <c r="H68" s="9"/>
+      <c r="A68" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" t="s">
+        <v>138</v>
+      </c>
+      <c r="E68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68">
+        <v>60</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I68" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B69" s="9"/>
-      <c r="H69" s="9"/>
+      <c r="A69" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" t="s">
+        <v>76</v>
+      </c>
+      <c r="D69" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69">
+        <v>60</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I69" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B70" s="9"/>
-      <c r="H70" s="9"/>
+      <c r="A70" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" t="s">
+        <v>138</v>
+      </c>
+      <c r="E70" t="s">
+        <v>88</v>
+      </c>
+      <c r="F70">
+        <v>60</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I70" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B71" s="9"/>
-      <c r="H71" s="9"/>
+      <c r="A71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
+      </c>
+      <c r="E71" t="s">
+        <v>88</v>
+      </c>
+      <c r="F71">
+        <v>60</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I71" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B72" s="9"/>
-      <c r="H72" s="9"/>
+      <c r="A72" t="s">
+        <v>112</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" t="s">
+        <v>76</v>
+      </c>
+      <c r="D72" t="s">
+        <v>138</v>
+      </c>
+      <c r="E72" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72">
+        <v>60</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I72" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B73" s="9"/>
-      <c r="H73" s="9"/>
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" t="s">
+        <v>138</v>
+      </c>
+      <c r="E73" t="s">
+        <v>88</v>
+      </c>
+      <c r="F73">
+        <v>60</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I73" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B74" s="9"/>
-      <c r="H74" s="9"/>
+      <c r="A74" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" t="s">
+        <v>138</v>
+      </c>
+      <c r="E74" t="s">
+        <v>88</v>
+      </c>
+      <c r="F74">
+        <v>60</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I74" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B75" s="9"/>
-      <c r="H75" s="9"/>
+      <c r="A75" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" t="s">
+        <v>76</v>
+      </c>
+      <c r="D75" t="s">
+        <v>138</v>
+      </c>
+      <c r="E75" t="s">
+        <v>88</v>
+      </c>
+      <c r="F75">
+        <v>60</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I75" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B76" s="9"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F97" s="9"/>
+      <c r="A76" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76" t="s">
+        <v>88</v>
+      </c>
+      <c r="F76">
+        <v>60</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" t="s">
+        <v>76</v>
+      </c>
+      <c r="D77" t="s">
+        <v>138</v>
+      </c>
+      <c r="E77" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77">
+        <v>60</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" t="s">
+        <v>138</v>
+      </c>
+      <c r="E78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78">
+        <v>60</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I78" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" t="s">
+        <v>76</v>
+      </c>
+      <c r="D79" t="s">
+        <v>138</v>
+      </c>
+      <c r="E79" t="s">
+        <v>88</v>
+      </c>
+      <c r="F79">
+        <v>60</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80" t="s">
+        <v>76</v>
+      </c>
+      <c r="D80" t="s">
+        <v>138</v>
+      </c>
+      <c r="E80" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80">
+        <v>60</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" t="s">
+        <v>76</v>
+      </c>
+      <c r="D81" t="s">
+        <v>138</v>
+      </c>
+      <c r="E81" t="s">
+        <v>88</v>
+      </c>
+      <c r="F81">
+        <v>60</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" t="s">
+        <v>76</v>
+      </c>
+      <c r="D82" t="s">
+        <v>138</v>
+      </c>
+      <c r="E82" t="s">
+        <v>88</v>
+      </c>
+      <c r="F82">
+        <v>60</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H82" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" t="s">
+        <v>76</v>
+      </c>
+      <c r="D83" t="s">
+        <v>138</v>
+      </c>
+      <c r="E83" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83">
+        <v>60</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H83" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" t="s">
+        <v>76</v>
+      </c>
+      <c r="D84" t="s">
+        <v>138</v>
+      </c>
+      <c r="E84" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84">
+        <v>60</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>125</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" t="s">
+        <v>76</v>
+      </c>
+      <c r="D85" t="s">
+        <v>138</v>
+      </c>
+      <c r="E85" t="s">
+        <v>88</v>
+      </c>
+      <c r="F85">
+        <v>60</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H85" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>126</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" t="s">
+        <v>76</v>
+      </c>
+      <c r="D86" t="s">
+        <v>138</v>
+      </c>
+      <c r="E86" t="s">
+        <v>88</v>
+      </c>
+      <c r="F86">
+        <v>33</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>127</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" t="s">
+        <v>76</v>
+      </c>
+      <c r="D87" t="s">
+        <v>138</v>
+      </c>
+      <c r="E87" t="s">
+        <v>88</v>
+      </c>
+      <c r="F87">
+        <v>33</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H87" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" t="s">
+        <v>76</v>
+      </c>
+      <c r="D88" t="s">
+        <v>138</v>
+      </c>
+      <c r="E88" t="s">
+        <v>88</v>
+      </c>
+      <c r="F88">
+        <v>33</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" t="s">
+        <v>76</v>
+      </c>
+      <c r="D89" t="s">
+        <v>138</v>
+      </c>
+      <c r="E89" t="s">
+        <v>88</v>
+      </c>
+      <c r="F89">
+        <v>33</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>130</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" t="s">
+        <v>138</v>
+      </c>
+      <c r="E90" t="s">
+        <v>88</v>
+      </c>
+      <c r="F90">
+        <v>33</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>131</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" t="s">
+        <v>76</v>
+      </c>
+      <c r="D91" t="s">
+        <v>138</v>
+      </c>
+      <c r="E91" t="s">
+        <v>88</v>
+      </c>
+      <c r="F91">
+        <v>33</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I91" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>132</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" t="s">
+        <v>76</v>
+      </c>
+      <c r="D92" t="s">
+        <v>138</v>
+      </c>
+      <c r="E92" t="s">
+        <v>88</v>
+      </c>
+      <c r="F92">
+        <v>33</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>133</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" t="s">
+        <v>138</v>
+      </c>
+      <c r="E93" t="s">
+        <v>88</v>
+      </c>
+      <c r="F93">
+        <v>33</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H93" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I93" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>134</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" t="s">
+        <v>76</v>
+      </c>
+      <c r="D94" t="s">
+        <v>138</v>
+      </c>
+      <c r="E94" t="s">
+        <v>88</v>
+      </c>
+      <c r="F94">
+        <v>33</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H94" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I94" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>135</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D95" t="s">
+        <v>138</v>
+      </c>
+      <c r="E95" t="s">
+        <v>88</v>
+      </c>
+      <c r="F95">
+        <v>33</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I95" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>136</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96" t="s">
+        <v>76</v>
+      </c>
+      <c r="D96" t="s">
+        <v>138</v>
+      </c>
+      <c r="E96" t="s">
+        <v>88</v>
+      </c>
+      <c r="F96">
+        <v>33</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H96" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I96" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>137</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C97" t="s">
+        <v>76</v>
+      </c>
+      <c r="D97" t="s">
+        <v>138</v>
+      </c>
+      <c r="E97" t="s">
+        <v>88</v>
+      </c>
+      <c r="F97">
+        <v>33</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H97" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I97" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F129" s="9"/>
@@ -4709,7 +5633,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="24"/>
     <col min="2" max="2" width="35.77734375" style="24" bestFit="1" customWidth="1"/>

</xml_diff>